<commit_message>
updated sprint backlog for end of day 3
</commit_message>
<xml_diff>
--- a/Sprint 2 Documentation/Sprint2Backlog.xlsx
+++ b/Sprint 2 Documentation/Sprint2Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2e22\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1dd4\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28BA9130-4C7A-4085-9D29-EA73FE42D94F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B0EC0C6-F381-4F56-B533-E162C6518CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>Backlog Task &amp; ID</t>
   </si>
@@ -88,12 +88,15 @@
     <t>AI</t>
   </si>
   <si>
+    <t>Update design of search function</t>
+  </si>
+  <si>
+    <t>AG, AN</t>
+  </si>
+  <si>
     <t>In-Progress</t>
   </si>
   <si>
-    <t>Update design of search function</t>
-  </si>
-  <si>
     <t>Reseach and follow accessibility guidelines</t>
   </si>
   <si>
@@ -115,16 +118,19 @@
     <t>WM</t>
   </si>
   <si>
-    <t>Map displays information about provider</t>
+    <t>Functionality for map to display information about provider</t>
+  </si>
+  <si>
+    <t>Map adapts to changing the page of results.</t>
   </si>
   <si>
     <t>21. As a customer, I can click a search result in the list and view it on the map</t>
   </si>
   <si>
-    <t>Map moves to location</t>
-  </si>
-  <si>
-    <t>Map zooms appropriately</t>
+    <t>Functionality for map to move to selected location</t>
+  </si>
+  <si>
+    <t>Functionality for map to zoom appropriately</t>
   </si>
   <si>
     <t>10. As a customer, I can set a price range for my search using a slider</t>
@@ -136,25 +142,31 @@
     <t>Pass variables from price slider to the results page</t>
   </si>
   <si>
+    <t>Add automatic value placement for double ended slider</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
     <t>11. As a customer, I can set a distance range for my search using a slider</t>
   </si>
   <si>
     <t xml:space="preserve">Create slider for distance range on search page </t>
   </si>
   <si>
-    <t>AG</t>
-  </si>
-  <si>
     <t>Pass variables from distance slider to the results page</t>
   </si>
   <si>
+    <t>Add automatic value placement for single ended slider</t>
+  </si>
+  <si>
     <t>16. As a customer, I can view service provider information page</t>
   </si>
   <si>
     <t>Update contact page design</t>
   </si>
   <si>
-    <t xml:space="preserve">Send a query by email implementation </t>
+    <t>JavaScript for email handling</t>
   </si>
   <si>
     <t>17. As an admin, I can login to an admin account</t>
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0174FFD9-7094-43F7-9D9D-5E73D5FB3BEA}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,32 +724,62 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>9</v>
       </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -748,10 +790,19 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="8" customFormat="1">
       <c r="A6" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8">
         <v>9</v>
@@ -762,7 +813,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -779,72 +830,166 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1">
-      <c r="A9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="8">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="8" customFormat="1">
+      <c r="A8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="8">
         <v>8</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F8" s="8">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4">
         <v>7</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F12" s="4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -853,49 +998,68 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="4" customFormat="1">
-      <c r="A16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="4">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4">
-        <v>4</v>
-      </c>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -909,12 +1073,14 @@
         <v>2</v>
       </c>
       <c r="G17" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -922,40 +1088,54 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="F18" s="7">
-        <v>2</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>4</v>
       </c>
       <c r="F19" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -972,52 +1152,88 @@
       <c r="H20">
         <v>0</v>
       </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="8" customFormat="1">
-      <c r="A22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="8">
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="8" customFormat="1">
+      <c r="A23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="8">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -1026,45 +1242,56 @@
         <v>4</v>
       </c>
       <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" s="4" customFormat="1">
-      <c r="A25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="I25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="4" customFormat="1">
+      <c r="A26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="4">
         <v>3</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F26" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1">
-      <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4">
+    <row r="29" spans="1:13" s="4" customFormat="1">
+      <c r="A29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F29" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="5"/>
@@ -1081,70 +1308,70 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1">
-      <c r="A31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="4">
+    <row r="31" spans="1:13">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:13" s="4" customFormat="1">
+      <c r="A32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4">
         <v>3</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F32" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:13">
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:13" s="4" customFormat="1">
-      <c r="A34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="4">
+    <row r="34" spans="1:13">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1">
+      <c r="A35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="4">
         <v>3</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F35" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="4" customFormat="1">
-      <c r="A37" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="4">
+    <row r="38" spans="1:13" s="4" customFormat="1">
+      <c r="A38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4">
         <v>2</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F38" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="4" customFormat="1">
-      <c r="A40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="F40" s="4">
+    <row r="41" spans="1:13" s="4" customFormat="1">
+      <c r="A41" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="F41" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="5"/>
@@ -1161,55 +1388,70 @@
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
     </row>
-    <row r="43" spans="1:13" s="4" customFormat="1">
-      <c r="A43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="F43" s="4">
+    <row r="43" spans="1:13">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" s="4" customFormat="1">
+      <c r="A44" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="3" customFormat="1">
-      <c r="A46" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" t="s">
-        <v>49</v>
+    <row r="47" spans="1:13" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1242,12 +1484,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1273,12 +1515,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15">

</xml_diff>

<commit_message>
added the TDD roadmap and updated the sprint backlog
</commit_message>
<xml_diff>
--- a/Sprint 2 Documentation/Sprint2Backlog.xlsx
+++ b/Sprint 2 Documentation/Sprint2Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2e22\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_828\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28BA9130-4C7A-4085-9D29-EA73FE42D94F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CFCF304-E3AD-4321-8C3D-DE5F1080EBDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Backlog Task &amp; ID</t>
   </si>
@@ -88,121 +88,133 @@
     <t>AI</t>
   </si>
   <si>
+    <t>Update design of search function</t>
+  </si>
+  <si>
+    <t>AG, AN</t>
+  </si>
+  <si>
+    <t>Reseach and follow accessibility guidelines</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>3. As a customer, I can search based on location</t>
+  </si>
+  <si>
+    <t>Finalise Live Location implementation</t>
+  </si>
+  <si>
+    <t>9. As a customer, I can view search results on a map</t>
+  </si>
+  <si>
+    <t>Integrate Map functionality with front-end</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>Functionality for map to display information about provider</t>
+  </si>
+  <si>
+    <t>Map adapts to changing the page of results.</t>
+  </si>
+  <si>
+    <t>21. As a customer, I can click a search result in the list and view it on the map</t>
+  </si>
+  <si>
+    <t>Functionality for map to move to selected location</t>
+  </si>
+  <si>
+    <t>Functionality for map to zoom appropriately</t>
+  </si>
+  <si>
+    <t>10. As a customer, I can set a price range for my search using a slider</t>
+  </si>
+  <si>
+    <t>Create slider for price range on search page</t>
+  </si>
+  <si>
+    <t>Pass variables from price slider to the results page</t>
+  </si>
+  <si>
+    <t>Add automatic value placement for double ended slider</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>11. As a customer, I can set a distance range for my search using a slider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create slider for distance range on search page </t>
+  </si>
+  <si>
+    <t>Pass variables from distance slider to the results page</t>
+  </si>
+  <si>
+    <t>Add automatic value placement for single ended slider</t>
+  </si>
+  <si>
+    <t>16. As a customer, I can view the contact page</t>
+  </si>
+  <si>
+    <t>Update contact page design</t>
+  </si>
+  <si>
+    <t>JS script pop up to notify the user</t>
+  </si>
+  <si>
+    <t>17. As an admin, I can login to an admin account</t>
+  </si>
+  <si>
+    <t>19. As an admin, I can add a new medical centre</t>
+  </si>
+  <si>
+    <t>20. As an admin, I can remove a medical centre</t>
+  </si>
+  <si>
+    <t>18. As an admin, I can edit details of a medical centre</t>
+  </si>
+  <si>
+    <t>7. As a customer, I can sort search results based on "best match"</t>
+  </si>
+  <si>
+    <t>5. As a customer, I can sort search results based on rating</t>
+  </si>
+  <si>
+    <t>15. As a customer, I can rate a medical centre</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Team Members unit of work (daily)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrius (AN) - </t>
+  </si>
+  <si>
+    <t>Alek (AR) -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amy (AG) - </t>
+  </si>
+  <si>
+    <t>Aylin (AI) -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William (WM) - </t>
+  </si>
+  <si>
+    <t>Calum (CW) -</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
     <t>In-Progress</t>
-  </si>
-  <si>
-    <t>Update design of search function</t>
-  </si>
-  <si>
-    <t>Reseach and follow accessibility guidelines</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>3. As a customer, I can search based on location</t>
-  </si>
-  <si>
-    <t>Finalise Live Location implementation</t>
-  </si>
-  <si>
-    <t>9. As a customer, I can view search results on a map</t>
-  </si>
-  <si>
-    <t>Integrate Map functionality with front-end</t>
-  </si>
-  <si>
-    <t>WM</t>
-  </si>
-  <si>
-    <t>Map displays information about provider</t>
-  </si>
-  <si>
-    <t>21. As a customer, I can click a search result in the list and view it on the map</t>
-  </si>
-  <si>
-    <t>Map moves to location</t>
-  </si>
-  <si>
-    <t>Map zooms appropriately</t>
-  </si>
-  <si>
-    <t>10. As a customer, I can set a price range for my search using a slider</t>
-  </si>
-  <si>
-    <t>Create slider for price range on search page</t>
-  </si>
-  <si>
-    <t>Pass variables from price slider to the results page</t>
-  </si>
-  <si>
-    <t>11. As a customer, I can set a distance range for my search using a slider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create slider for distance range on search page </t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>Pass variables from distance slider to the results page</t>
-  </si>
-  <si>
-    <t>16. As a customer, I can view service provider information page</t>
-  </si>
-  <si>
-    <t>Update contact page design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Send a query by email implementation </t>
-  </si>
-  <si>
-    <t>17. As an admin, I can login to an admin account</t>
-  </si>
-  <si>
-    <t>19. As an admin, I can add a new medical centre</t>
-  </si>
-  <si>
-    <t>20. As an admin, I can remove a medical centre</t>
-  </si>
-  <si>
-    <t>18. As an admin, I can edit details of a medical centre</t>
-  </si>
-  <si>
-    <t>7. As a customer, I can sort search results based on "best match"</t>
-  </si>
-  <si>
-    <t>5. As a customer, I can sort search results based on rating</t>
-  </si>
-  <si>
-    <t>15. As a customer, I can rate a medical centre</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Team Members unit of work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrius (AN) - </t>
-  </si>
-  <si>
-    <t>Alek (AR) -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amy (AG) - </t>
-  </si>
-  <si>
-    <t>Aylin (AI) -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William (WM) - </t>
-  </si>
-  <si>
-    <t>Calum (CW) -</t>
-  </si>
-  <si>
-    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0174FFD9-7094-43F7-9D9D-5E73D5FB3BEA}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,21 +724,51 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>9</v>
       </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -737,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -746,6 +788,12 @@
         <v>2</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>0</v>
       </c>
     </row>
@@ -779,21 +827,53 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1">
-      <c r="A9" s="8" t="s">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="8" customFormat="1">
+      <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B8" s="8">
         <v>8</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F8" s="8">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -802,50 +882,97 @@
         <v>14</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4">
         <v>7</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F12" s="4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
@@ -853,49 +980,63 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="4" customFormat="1">
-      <c r="A16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="4">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4">
-        <v>4</v>
-      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -909,50 +1050,66 @@
         <v>2</v>
       </c>
       <c r="G17" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="F18" s="7">
-        <v>2</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4">
         <v>4</v>
       </c>
       <c r="F19" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>36</v>
@@ -972,52 +1129,88 @@
       <c r="H20">
         <v>0</v>
       </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="8" customFormat="1">
-      <c r="A22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="8">
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="8" customFormat="1">
+      <c r="A23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="8">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -1026,45 +1219,62 @@
         <v>4</v>
       </c>
       <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="4" customFormat="1">
-      <c r="A25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="4">
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>1.5</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="4" customFormat="1">
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4">
         <v>3</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F26" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1">
-      <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4">
+    <row r="29" spans="1:13" s="4" customFormat="1">
+      <c r="A29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F29" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="5"/>
@@ -1081,70 +1291,70 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1">
-      <c r="A31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="4">
+    <row r="31" spans="1:13">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:13" s="4" customFormat="1">
+      <c r="A32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="4">
         <v>3</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F32" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:13">
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:13" s="4" customFormat="1">
-      <c r="A34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="4">
+    <row r="34" spans="1:13">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1">
+      <c r="A35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="4">
         <v>3</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F35" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="4" customFormat="1">
-      <c r="A37" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="4">
+    <row r="38" spans="1:13" s="4" customFormat="1">
+      <c r="A38" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="4">
         <v>2</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F38" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="4" customFormat="1">
-      <c r="A40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="F40" s="4">
+    <row r="41" spans="1:13" s="4" customFormat="1">
+      <c r="A41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="F41" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="5"/>
@@ -1161,55 +1371,88 @@
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
     </row>
-    <row r="43" spans="1:13" s="4" customFormat="1">
-      <c r="A43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="F43" s="4">
+    <row r="43" spans="1:13">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" s="4" customFormat="1">
+      <c r="A44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="3" customFormat="1">
-      <c r="A46" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+    <row r="47" spans="1:13" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
+        <v>53</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+        <v>55</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1242,12 +1485,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1273,12 +1516,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15">

</xml_diff>